<commit_message>
3 CDAs von Dominik + Korrekturen
</commit_message>
<xml_diff>
--- a/cda_basismodul/CDA Beispielpatienten.xlsx
+++ b/cda_basismodul/CDA Beispielpatienten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="135">
   <si>
     <t>Patient</t>
   </si>
@@ -366,24 +366,6 @@
     <t>Tod</t>
   </si>
   <si>
-    <t>Schädelhirntrauma</t>
-  </si>
-  <si>
-    <t>ICB</t>
-  </si>
-  <si>
-    <t>Verkehrsmittelunfall</t>
-  </si>
-  <si>
-    <t>Rippenserienfraktur</t>
-  </si>
-  <si>
-    <t>Hämatothorax</t>
-  </si>
-  <si>
-    <t>Kardiogener Schock</t>
-  </si>
-  <si>
     <t>Vertragsarzt</t>
   </si>
   <si>
@@ -418,6 +400,27 @@
   </si>
   <si>
     <t>I21</t>
+  </si>
+  <si>
+    <t>I26.9</t>
+  </si>
+  <si>
+    <t>R57.0</t>
+  </si>
+  <si>
+    <t>S06.79!</t>
+  </si>
+  <si>
+    <t>I61.9</t>
+  </si>
+  <si>
+    <t>V99!</t>
+  </si>
+  <si>
+    <t>S22.40</t>
+  </si>
+  <si>
+    <t>S27.1</t>
   </si>
 </sst>
 </file>
@@ -463,10 +466,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -770,13 +773,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="BZ1" workbookViewId="0">
+      <selection activeCell="CU4" sqref="CU4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1047,557 +1051,638 @@
       </c>
     </row>
     <row r="2" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>19858</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>42193</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>0.70208333333333339</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>0.70486111111111116</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="5">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2">
+      <c r="H2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3">
         <v>651</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="5">
         <v>0.625</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="3">
         <v>1</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="3">
         <v>0</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="S2" t="s">
+      <c r="R2" s="3"/>
+      <c r="S2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="U2" s="4">
+      <c r="T2" s="3"/>
+      <c r="U2" s="3">
         <v>12</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="3">
         <v>94</v>
       </c>
-      <c r="W2" s="4">
+      <c r="W2" s="3">
         <v>85</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="3">
         <v>131</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Y2" s="3">
         <v>1</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="Z2" s="3">
         <v>1</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AA2" s="3">
         <v>1</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="3">
         <v>3</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AG2" s="4">
+      <c r="AG2" s="3">
         <v>36.700000000000003</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="3">
         <v>0</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AI2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AK2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL2" s="2">
+      <c r="AK2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL2" s="5">
         <v>0.71180555555555547</v>
       </c>
-      <c r="AM2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AO2" s="2">
+      <c r="AM2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO2" s="5">
         <v>0.71388888888888891</v>
       </c>
-      <c r="AP2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR2" s="2">
+      <c r="AP2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR2" s="5">
         <v>0.72569444444444453</v>
       </c>
-      <c r="AS2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AU2" s="2">
+      <c r="AS2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU2" s="5">
         <v>0.71527777777777779</v>
       </c>
-      <c r="AV2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BA2" s="3">
+      <c r="AV2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX2" s="3"/>
+      <c r="AY2" s="3"/>
+      <c r="AZ2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA2" s="6">
         <v>0.71875</v>
       </c>
-      <c r="BB2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BP2" s="2">
+      <c r="BB2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BD2" s="3"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="3"/>
+      <c r="BI2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ2" s="3"/>
+      <c r="BK2" s="3"/>
+      <c r="BL2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BM2" s="3"/>
+      <c r="BN2" s="3"/>
+      <c r="BO2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BP2" s="5">
         <v>0.73263888888888884</v>
       </c>
-      <c r="BQ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>85</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>121</v>
-      </c>
-      <c r="CI2" s="6">
+      <c r="BQ2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BS2" s="3"/>
+      <c r="BT2" s="3"/>
+      <c r="BU2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BV2" s="3"/>
+      <c r="BW2" s="3"/>
+      <c r="BX2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY2" s="3"/>
+      <c r="BZ2" s="3"/>
+      <c r="CA2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="CB2" s="3"/>
+      <c r="CC2" s="3"/>
+      <c r="CD2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="CE2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="CF2" s="3"/>
+      <c r="CG2" s="3"/>
+      <c r="CH2" s="3"/>
+      <c r="CI2" s="5">
         <v>0.86458333333333337</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="CJ2" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>34914</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>42193</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="5">
         <v>0.33402777777777781</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="5">
         <v>0.33402777777777781</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="5">
         <v>0.33680555555555558</v>
       </c>
-      <c r="H3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3">
+      <c r="H3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="3">
         <v>802</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="5">
         <v>0.30138888888888887</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="3">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="3">
         <v>0</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="S3" t="s">
+      <c r="R3" s="3"/>
+      <c r="S3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="U3">
+      <c r="T3" s="3"/>
+      <c r="U3" s="3">
         <v>14</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="3">
         <v>98</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="3">
         <v>105</v>
       </c>
-      <c r="X3">
-        <v>95</v>
-      </c>
-      <c r="Y3">
+      <c r="X3" s="3">
+        <v>95</v>
+      </c>
+      <c r="Y3" s="3">
         <v>1</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="3">
         <v>1</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="3">
         <v>1</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="3">
         <v>3</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="3">
         <v>35.5</v>
       </c>
-      <c r="AH3">
+      <c r="AH3" s="3">
         <v>0</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AK3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL3" s="2">
+      <c r="AK3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL3" s="5">
         <v>0.34722222222222227</v>
       </c>
-      <c r="AM3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AO3" s="2">
+      <c r="AM3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO3" s="5">
         <v>0.34722222222222227</v>
       </c>
-      <c r="AP3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX3" s="2">
+      <c r="AP3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU3" s="3"/>
+      <c r="AV3" s="3"/>
+      <c r="AW3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX3" s="5">
         <v>0.34027777777777773</v>
       </c>
-      <c r="AY3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>95</v>
-      </c>
-      <c r="BA3" s="2">
+      <c r="AY3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA3" s="5">
         <v>0.34027777777777773</v>
       </c>
-      <c r="BB3" t="s">
-        <v>95</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>95</v>
-      </c>
-      <c r="BD3" s="2">
+      <c r="BB3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BC3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD3" s="5">
         <v>0.35069444444444442</v>
       </c>
-      <c r="BE3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>95</v>
-      </c>
-      <c r="BJ3" s="2">
+      <c r="BE3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BF3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
+      <c r="BI3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BJ3" s="5">
         <v>0.35416666666666669</v>
       </c>
-      <c r="BK3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>87</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>116</v>
-      </c>
-      <c r="CE3" t="s">
+      <c r="BK3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BL3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BM3" s="3"/>
+      <c r="BN3" s="3"/>
+      <c r="BO3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BP3" s="3"/>
+      <c r="BQ3" s="3"/>
+      <c r="BR3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BS3" s="3"/>
+      <c r="BT3" s="3"/>
+      <c r="BU3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BV3" s="3"/>
+      <c r="BW3" s="3"/>
+      <c r="BX3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY3" s="3"/>
+      <c r="BZ3" s="3"/>
+      <c r="CA3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="CB3" s="3"/>
+      <c r="CC3" s="3"/>
+      <c r="CD3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="CE3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="CF3" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="CG3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CH3" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CI3" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="CJ3" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="CF3" t="s">
-        <v>118</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>119</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>120</v>
-      </c>
-      <c r="CI3" s="2">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>11658</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>42193</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>0.86388888888888893</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>0.86458333333333337</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
         <v>0.86458333333333337</v>
       </c>
-      <c r="H4" t="s">
-        <v>87</v>
-      </c>
-      <c r="L4">
+      <c r="H4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3">
         <v>1</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="5">
         <v>0.83263888888888893</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="3">
         <v>1</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="3">
         <v>4</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="3">
         <v>12</v>
       </c>
-      <c r="Y4">
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3">
         <v>1</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="3">
         <v>1</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="3">
         <v>1</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="3">
         <v>3</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AC4" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AE4" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AF4" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="3">
         <v>35.700000000000003</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="3">
         <v>0</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AI4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AK4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AO4" s="2">
+      <c r="AK4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO4" s="5">
         <v>0.87291666666666667</v>
       </c>
-      <c r="AP4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>95</v>
-      </c>
-      <c r="BA4" s="2">
+      <c r="AP4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU4" s="3"/>
+      <c r="AV4" s="3"/>
+      <c r="AW4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX4" s="3"/>
+      <c r="AY4" s="3"/>
+      <c r="AZ4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA4" s="5">
         <v>0.87152777777777779</v>
       </c>
-      <c r="BB4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BL4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BR4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BU4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA4" t="s">
-        <v>87</v>
-      </c>
-      <c r="CD4" t="s">
-        <v>132</v>
-      </c>
-      <c r="CE4" t="s">
-        <v>133</v>
-      </c>
-      <c r="CI4" s="2">
+      <c r="BB4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BC4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BD4" s="3"/>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG4" s="3"/>
+      <c r="BH4" s="3"/>
+      <c r="BI4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ4" s="3"/>
+      <c r="BK4" s="3"/>
+      <c r="BL4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BM4" s="3"/>
+      <c r="BN4" s="3"/>
+      <c r="BO4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BP4" s="3"/>
+      <c r="BQ4" s="3"/>
+      <c r="BR4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BS4" s="3"/>
+      <c r="BT4" s="3"/>
+      <c r="BU4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BV4" s="3"/>
+      <c r="BW4" s="3"/>
+      <c r="BX4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY4" s="3"/>
+      <c r="BZ4" s="3"/>
+      <c r="CA4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="CB4" s="3"/>
+      <c r="CC4" s="3"/>
+      <c r="CD4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="CE4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="CF4" s="3"/>
+      <c r="CG4" s="3"/>
+      <c r="CH4" s="3"/>
+      <c r="CI4" s="5">
         <v>0.88680555555555562</v>
       </c>
-      <c r="CJ4" t="s">
+      <c r="CJ4" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1699,10 +1784,10 @@
         <v>2</v>
       </c>
       <c r="AI5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="AJ5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="AK5" t="s">
         <v>95</v>
@@ -1774,13 +1859,13 @@
         <v>87</v>
       </c>
       <c r="CD5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="CI5" s="2">
         <v>0.77986111111111101</v>
       </c>
       <c r="CJ5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.25">
@@ -1872,10 +1957,10 @@
         <v>3</v>
       </c>
       <c r="AI6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="AJ6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="AK6" t="s">
         <v>87</v>
@@ -1929,13 +2014,13 @@
         <v>87</v>
       </c>
       <c r="CD6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="CI6" s="2">
         <v>0.83333333333333337</v>
       </c>
       <c r="CJ6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:88" x14ac:dyDescent="0.25">
@@ -2036,10 +2121,10 @@
         <v>6</v>
       </c>
       <c r="AI7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="AJ7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="AK7" t="s">
         <v>95</v>
@@ -2100,16 +2185,16 @@
         <v>87</v>
       </c>
       <c r="CD7" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="CE7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="CI7" s="2">
         <v>4.5138888888888888E-2</v>
       </c>
       <c r="CJ7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:88" x14ac:dyDescent="0.25">
@@ -2138,7 +2223,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>